<commit_message>
Remove extra TS code block rows from operations workbook
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1034,484 +1034,7 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>Exact TS code blocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>create.paragraph (docapi:create-paragraph)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
-import { dirname } from 'node:path';
-import { get as httpsGet } from 'node:https';
-import { get as httpGet } from 'node:http';
-import { describe, expect, it } from 'vitest';
-import { createDocumentApi } from '@superdoc/document-api';
-import { Editor } from '../core/Editor.js';
-import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
-function toRawGithubUrl(input: string): string {
-  if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
-}
-function isHttpSource(input: string): boolean {
-  return input.startsWith('http://') || input.startsWith('https://');
-}
-async function loadSource(source: string): Promise&lt;string | Buffer&gt; {
-  if (!isHttpSource(source)) return source;
-  const url = toRawGithubUrl(source);
-  const client = url.startsWith('https://') ? httpsGet : httpGet;
-  return new Promise&lt;Buffer&gt;((resolveBuffer, reject) =&gt; {
-    client(url, (res) =&gt; {
-      const status = res.statusCode ?? 0;
-      if (status &gt;= 300 &amp;&amp; status &lt; 400 &amp;&amp; res.headers.location) {
-        loadSource(res.headers.location)
-          .then((next) =&gt; {
-            if (typeof next === 'string') {
-              reject(new Error(`Redirect resolved to non-buffer source: ${res.headers.location}`));
-              return;
-            }
-            resolveBuffer(next);
-          })
-          .catch(reject);
-        return;
-      }
-      if (status &lt; 200 || status &gt;= 300) {
-        reject(new Error(`Failed to fetch source DOCX (${status}): ${url}`));
-        return;
-      }
-      const chunks: Buffer[] = [];
-      res.on('data', (chunk) =&gt; chunks.push(Buffer.isBuffer(chunk) ? chunk : Buffer.from(chunk)));
-      res.on('end', () =&gt; resolveBuffer(Buffer.concat(chunks)));
-      res.on('error', reject);
-    }).on('error', reject);
-  });
-}
-describe('docapi create paragraph', () =&gt; {
-  it('creates a paragraph via create.paragraph and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
-    const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-create-paragraph-output.docx';
-    const paragraphText = process.env.DOCAPI_PARAGRAPH_TEXT ?? 'apples, bananas, mangoes';
-    await mkdir(dirname(outputPath), { recursive: true });
-    const openedSource = await loadSource(source);
-    const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
-    try {
-      editor.commands.selectAll();
-      editor.commands.deleteSelection();
-      const doc = createDocumentApi(assembleDocumentApiAdapters(editor));
-      const result = doc.create.paragraph({
-        text: paragraphText,
-      });
-      if (!result.success) {
-        throw new Error(`Failed to create paragraph: ${result.failure?.message ?? 'unknown error'}`);
-      }
-      await editor.saveTo(outputPath);
-      const outputStats = await stat(outputPath);
-      expect(outputStats.size).toBeGreaterThan(0);
-      console.log(`DOCX written: ${outputPath}`);
-    } finally {
-      editor.destroy();
-    }
-  });
-});
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>create.heading (docapi:create-heading)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
-import { dirname } from 'node:path';
-import { get as httpsGet } from 'node:https';
-import { get as httpGet } from 'node:http';
-import { describe, expect, it } from 'vitest';
-import { createDocumentApi } from '@superdoc/document-api';
-import { Editor } from '../core/Editor.js';
-import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
-function toRawGithubUrl(input: string): string {
-  if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
-}
-function isHttpSource(input: string): boolean {
-  return input.startsWith('http://') || input.startsWith('https://');
-}
-async function loadSource(source: string): Promise&lt;string | Buffer&gt; {
-  if (!isHttpSource(source)) return source;
-  const url = toRawGithubUrl(source);
-  const client = url.startsWith('https://') ? httpsGet : httpGet;
-  return new Promise&lt;Buffer&gt;((resolveBuffer, reject) =&gt; {
-    client(url, (res) =&gt; {
-      const status = res.statusCode ?? 0;
-      if (status &gt;= 300 &amp;&amp; status &lt; 400 &amp;&amp; res.headers.location) {
-        loadSource(res.headers.location)
-          .then((next) =&gt; {
-            if (typeof next === 'string') {
-              reject(new Error(`Redirect resolved to non-buffer source: ${res.headers.location}`));
-              return;
-            }
-            resolveBuffer(next);
-          })
-          .catch(reject);
-        return;
-      }
-      if (status &lt; 200 || status &gt;= 300) {
-        reject(new Error(`Failed to fetch source DOCX (${status}): ${url}`));
-        return;
-      }
-      const chunks: Buffer[] = [];
-      res.on('data', (chunk) =&gt; chunks.push(Buffer.isBuffer(chunk) ? chunk : Buffer.from(chunk)));
-      res.on('end', () =&gt; resolveBuffer(Buffer.concat(chunks)));
-      res.on('error', reject);
-    }).on('error', reject);
-  });
-}
-describe('docapi create heading', () =&gt; {
-  it('creates a heading via create.heading and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
-    const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-create-heading-output.docx';
-    const headingText = process.env.DOCAPI_HEADING_TEXT ?? 'FRUIT';
-    const headingLevelRaw = Number.parseInt(process.env.DOCAPI_HEADING_LEVEL ?? '1', 10);
-    const headingLevel = Number.isFinite(headingLevelRaw) ? Math.max(1, Math.min(6, headingLevelRaw)) : 1;
-    await mkdir(dirname(outputPath), { recursive: true });
-    const openedSource = await loadSource(source);
-    const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
-    try {
-      editor.commands.selectAll();
-      editor.commands.deleteSelection();
-      const doc = createDocumentApi(assembleDocumentApiAdapters(editor));
-      const result = doc.create.heading({
-        level: headingLevel as 1 | 2 | 3 | 4 | 5 | 6,
-        text: headingText,
-      });
-      if (!result.success) {
-        throw new Error(`Failed to create heading: ${result.failure?.message ?? 'unknown error'}`);
-      }
-      await editor.saveTo(outputPath);
-      const outputStats = await stat(outputPath);
-      expect(outputStats.size).toBeGreaterThan(0);
-      console.log(`DOCX written: ${outputPath}`);
-    } finally {
-      editor.destroy();
-    }
-  });
-});
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>create.table (docapi:create-table)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
-import { dirname } from 'node:path';
-import { get as httpsGet } from 'node:https';
-import { get as httpGet } from 'node:http';
-import { describe, expect, it } from 'vitest';
-import { createDocumentApi } from '@superdoc/document-api';
-import { Editor } from '../core/Editor.js';
-import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
-function toRawGithubUrl(input: string): string {
-  if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
-}
-function isHttpSource(input: string): boolean {
-  return input.startsWith('http://') || input.startsWith('https://');
-}
-async function loadSource(source: string): Promise&lt;string | Buffer&gt; {
-  if (!isHttpSource(source)) return source;
-  const url = toRawGithubUrl(source);
-  const client = url.startsWith('https://') ? httpsGet : httpGet;
-  return new Promise&lt;Buffer&gt;((resolveBuffer, reject) =&gt; {
-    client(url, (res) =&gt; {
-      const status = res.statusCode ?? 0;
-      if (status &gt;= 300 &amp;&amp; status &lt; 400 &amp;&amp; res.headers.location) {
-        loadSource(res.headers.location)
-          .then((next) =&gt; {
-            if (typeof next === 'string') {
-              reject(new Error(`Redirect resolved to non-buffer source: ${res.headers.location}`));
-              return;
-            }
-            resolveBuffer(next);
-          })
-          .catch(reject);
-        return;
-      }
-      if (status &lt; 200 || status &gt;= 300) {
-        reject(new Error(`Failed to fetch source DOCX (${status}): ${url}`));
-        return;
-      }
-      const chunks: Buffer[] = [];
-      res.on('data', (chunk) =&gt; chunks.push(Buffer.isBuffer(chunk) ? chunk : Buffer.from(chunk)));
-      res.on('end', () =&gt; resolveBuffer(Buffer.concat(chunks)));
-      res.on('error', reject);
-    }).on('error', reject);
-  });
-}
-describe('docapi create table', () =&gt; {
-  it('creates a table via create.table and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
-    const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-create-table-output.docx';
-    const rowsRaw = Number.parseInt(process.env.DOCAPI_TABLE_ROWS ?? '3', 10);
-    const columnsRaw = Number.parseInt(process.env.DOCAPI_TABLE_COLUMNS ?? '3', 10);
-    const rows = Number.isFinite(rowsRaw) ? Math.max(1, rowsRaw) : 3;
-    const columns = Number.isFinite(columnsRaw) ? Math.max(1, columnsRaw) : 3;
-    await mkdir(dirname(outputPath), { recursive: true });
-    const openedSource = await loadSource(source);
-    const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
-    try {
-      editor.commands.selectAll();
-      editor.commands.deleteSelection();
-      const doc = createDocumentApi(assembleDocumentApiAdapters(editor));
-      const result = doc.create.table({
-        rows,
-        columns,
-      });
-      if (!result.success) {
-        throw new Error(`Failed to create table: ${result.failure?.message ?? 'unknown error'}`);
-      }
-      await editor.saveTo(outputPath);
-      const outputStats = await stat(outputPath);
-      expect(outputStats.size).toBeGreaterThan(0);
-      console.log(`DOCX written: ${outputPath}`);
-    } finally {
-      editor.destroy();
-    }
-  });
-});
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>insert (docapi:insert)</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
-import { dirname } from 'node:path';
-import { get as httpsGet } from 'node:https';
-import { get as httpGet } from 'node:http';
-import { describe, expect, it } from 'vitest';
-import { createDocumentApi } from '@superdoc/document-api';
-import { Editor } from '../core/Editor.js';
-import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
-function toRawGithubUrl(input: string): string {
-  if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
-}
-function isHttpSource(input: string): boolean {
-  return input.startsWith('http://') || input.startsWith('https://');
-}
-async function loadSource(source: string): Promise&lt;string | Buffer&gt; {
-  if (!isHttpSource(source)) return source;
-  const url = toRawGithubUrl(source);
-  const client = url.startsWith('https://') ? httpsGet : httpGet;
-  return new Promise&lt;Buffer&gt;((resolveBuffer, reject) =&gt; {
-    client(url, (res) =&gt; {
-      const status = res.statusCode ?? 0;
-      if (status &gt;= 300 &amp;&amp; status &lt; 400 &amp;&amp; res.headers.location) {
-        loadSource(res.headers.location)
-          .then((next) =&gt; {
-            if (typeof next === 'string') {
-              reject(new Error(`Redirect resolved to non-buffer source: ${res.headers.location}`));
-              return;
-            }
-            resolveBuffer(next);
-          })
-          .catch(reject);
-        return;
-      }
-      if (status &lt; 200 || status &gt;= 300) {
-        reject(new Error(`Failed to fetch source DOCX (${status}): ${url}`));
-        return;
-      }
-      const chunks: Buffer[] = [];
-      res.on('data', (chunk) =&gt; chunks.push(Buffer.isBuffer(chunk) ? chunk : Buffer.from(chunk)));
-      res.on('end', () =&gt; resolveBuffer(Buffer.concat(chunks)));
-      res.on('error', reject);
-    }).on('error', reject);
-  });
-}
-describe('docapi insert', () =&gt; {
-  it('seeds content via insert and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
-    const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-insert-output.docx';
-    const insertText = process.env.DOCAPI_INSERT_TEXT ?? 'Seed content for follow-up operations.';
-    await mkdir(dirname(outputPath), { recursive: true });
-    const openedSource = await loadSource(source);
-    const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
-    try {
-      editor.commands.selectAll();
-      editor.commands.deleteSelection();
-      const doc = createDocumentApi(assembleDocumentApiAdapters(editor));
-      const result = doc.insert({ text: insertText });
-      if (!result.success) {
-        throw new Error(`Failed to insert text: ${result.failure?.message ?? 'unknown error'}`);
-      }
-      await editor.saveTo(outputPath);
-      const outputStats = await stat(outputPath);
-      expect(outputStats.size).toBeGreaterThan(0);
-      console.log(`DOCX written: ${outputPath}`);
-    } finally {
-      editor.destroy();
-    }
-  });
-});
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>lists.insert (docapi:lists-insert)</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
-import { dirname } from 'node:path';
-import { get as httpsGet } from 'node:https';
-import { get as httpGet } from 'node:http';
-import { describe, expect, it } from 'vitest';
-import { createDocumentApi } from '@superdoc/document-api';
-import { Editor } from '../core/Editor.js';
-import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
-function toRawGithubUrl(input: string): string {
-  if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
-}
-function isHttpSource(input: string): boolean {
-  return input.startsWith('http://') || input.startsWith('https://');
-}
-async function loadSource(source: string): Promise&lt;string | Buffer&gt; {
-  if (!isHttpSource(source)) return source;
-  const url = toRawGithubUrl(source);
-  const client = url.startsWith('https://') ? httpsGet : httpGet;
-  return new Promise&lt;Buffer&gt;((resolveBuffer, reject) =&gt; {
-    client(url, (res) =&gt; {
-      const status = res.statusCode ?? 0;
-      if (status &gt;= 300 &amp;&amp; status &lt; 400 &amp;&amp; res.headers.location) {
-        loadSource(res.headers.location)
-          .then((next) =&gt; {
-            if (typeof next === 'string') {
-              reject(new Error(`Redirect resolved to non-buffer source: ${res.headers.location}`));
-              return;
-            }
-            resolveBuffer(next);
-          })
-          .catch(reject);
-        return;
-      }
-      if (status &lt; 200 || status &gt;= 300) {
-        reject(new Error(`Failed to fetch source DOCX (${status}): ${url}`));
-        return;
-      }
-      const chunks: Buffer[] = [];
-      res.on('data', (chunk) =&gt; chunks.push(Buffer.isBuffer(chunk) ? chunk : Buffer.from(chunk)));
-      res.on('end', () =&gt; resolveBuffer(Buffer.concat(chunks)));
-      res.on('error', reject);
-    }).on('error', reject);
-  });
-}
-describe('docapi lists.insert', () =&gt; {
-  it('inserts a list item after seeding an initial list item target', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
-    const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-lists-insert-output.docx';
-    const firstItemText = process.env.DOCAPI_LIST_SEED_TEXT ?? 'Yabba';
-    const insertedItemText = process.env.DOCAPI_ITEM_TEXT ?? 'Dabba';
-    await mkdir(dirname(outputPath), { recursive: true });
-    const openedSource = await loadSource(source);
-    const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
-    try {
-      editor.commands.selectAll();
-      editor.commands.deleteSelection();
-      editor.commands.insertContent(firstItemText, { contentType: 'text' });
-      const toggled = editor.commands.toggleOrderedList?.();
-      if (!toggled) {
-        throw new Error('Failed to create starter ordered list item in source document.');
-      }
-      const doc = createDocumentApi(assembleDocumentApiAdapters(editor));
-      const listItems = doc.lists.list();
-      const firstItem = listItems.items[0]?.address;
-      if (!firstItem) {
-        throw new Error('Failed to resolve starter list item target for lists.insert.');
-      }
-      const result = doc.lists.insert({
-        target: firstItem,
-        position: 'after',
-        text: insertedItemText,
-      });
-      if (!result.success) {
-        throw new Error(`Failed to insert list item: ${result.failure?.message ?? 'unknown error'}`);
-      }
-      await editor.saveTo(outputPath);
-      const outputStats = await stat(outputPath);
-      expect(outputStats.size).toBeGreaterThan(0);
-      console.log(`DOCX written: ${outputPath}`);
-    } finally {
-      editor.destroy();
-    }
-  });
-});
-</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A22:F22"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add XML tags added/updated column to operations workbook
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,7 @@
     <col width="58" customWidth="1" min="4" max="4"/>
     <col width="120" customWidth="1" min="5" max="5"/>
     <col width="95" customWidth="1" min="6" max="6"/>
+    <col width="110" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,6 +469,11 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Script</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>XML tags added/updated (comma-separated)</t>
         </is>
       </c>
     </row>
@@ -577,6 +583,11 @@
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-create-paragraph-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-paragraph</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>
@@ -689,6 +700,11 @@
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-create-heading-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-heading</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:pStyle,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>
@@ -804,6 +820,11 @@
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-table</t>
         </is>
       </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:bottom,w:color,w:gridCol,w:ind,w:left,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:start,w:style,w:tbl,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:bottom,w:color,w:ind,w:left,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:style,w:styles,w:top,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -911,6 +932,11 @@
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:insert</t>
         </is>
       </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -1033,6 +1059,11 @@
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-insert</t>
         </is>
       </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ilvl,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numId,w:numPr,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:tmpl,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:color,w:ilvl,w:ind,w:name,w:numPr,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Split XML diff into Added/Updated properties columns
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,8 @@
     <col width="58" customWidth="1" min="4" max="4"/>
     <col width="120" customWidth="1" min="5" max="5"/>
     <col width="95" customWidth="1" min="6" max="6"/>
-    <col width="110" customWidth="1" min="7" max="7"/>
+    <col width="70" customWidth="1" min="7" max="7"/>
+    <col width="70" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -473,7 +474,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>XML tags added/updated (comma-separated)</t>
+          <t>Added XML properties</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Updated XML properties</t>
         </is>
       </c>
     </row>
@@ -587,7 +593,12 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>
@@ -704,7 +715,12 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:pStyle,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:pStyle,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>
@@ -822,7 +838,12 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:bottom,w:color,w:gridCol,w:ind,w:left,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:start,w:style,w:tbl,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:bottom,w:color,w:ind,w:left,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:style,w:styles,w:top,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:bottom,w:color,w:gridCol,w:ind,w:left,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:start,w:style,w:tbl,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr,w:u,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>Properties,w:basedOn,w:body,w:bottom,w:color,w:ind,w:left,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:style,w:styles,w:top,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>
@@ -934,7 +955,12 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Properties,w:basedOn,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1087,12 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>added:Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ilvl,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numId,w:numPr,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:tmpl,w:u,w:uiPriority,w:unhideWhenUsed | updated:Properties,w:basedOn,w:body,w:color,w:ilvl,w:ind,w:name,w:numPr,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ilvl,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numId,w:numPr,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:tmpl,w:u,w:uiPriority,w:unhideWhenUsed</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Properties,w:basedOn,w:body,w:color,w:ilvl,w:ind,w:name,w:numPr,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove non-tag property token from XML columns
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -593,7 +593,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:pStyle,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:pStyle,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -838,7 +838,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:bottom,w:color,w:gridCol,w:ind,w:left,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:start,w:style,w:tbl,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr,w:u,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:bottom,w:color,w:gridCol,w:ind,w:left,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:start,w:style,w:tbl,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Properties,lpwstr,property,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ilvl,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numId,w:numPr,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:tmpl,w:u,w:uiPriority,w:unhideWhenUsed</t>
+          <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ilvl,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numId,w:numPr,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:tmpl,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Update workbook scripts to Starting files Blank.docx path
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
+          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-create-paragraph-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-paragraph</t>
         </is>
@@ -708,7 +708,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
+          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-create-heading-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-heading</t>
         </is>
@@ -831,7 +831,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
+          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-create-table-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-table</t>
         </is>
@@ -948,7 +948,7 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
+          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-insert-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:insert</t>
         </is>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx" \
+          <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Downloads/docapi-lists-insert-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-insert</t>
         </is>

</xml_diff>

<commit_message>
Add namespace column to docapi operations workbook
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,7 +432,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
     <col width="26" customWidth="1" min="3" max="3"/>
     <col width="52" customWidth="1" min="4" max="4"/>
     <col width="110" customWidth="1" min="5" max="5"/>
@@ -449,35 +449,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Namespace</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Program</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Requires existing target</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Requirement details</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Actual TS code that is used in that program</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Script</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Added XML properties</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Updated XML properties</t>
         </is>
@@ -491,20 +496,25 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
+          <t>create</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
           <t>docapi:create-paragraph</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Can create from blank document; no existing node target required.</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -584,19 +594,19 @@
 </t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-create-paragraph-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-paragraph</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
@@ -610,20 +620,25 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>create</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
           <t>docapi:create-heading</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Can create from blank document; no existing node target required.</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -706,19 +721,19 @@
 </t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-create-heading-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-heading</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:pStyle,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>Properties,w:basedOn,w:body,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
@@ -732,20 +747,25 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
+          <t>create</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
           <t>docapi:create-table</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Can create from blank document; no existing node target required.</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -829,19 +849,19 @@
 </t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-create-table-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:create-table</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:bottom,w:color,w:gridCol,w:ind,w:left,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:start,w:style,w:tbl,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>Properties,w:basedOn,w:body,w:bottom,w:color,w:ind,w:left,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:right,w:rsid,w:style,w:styles,w:top,w:uiPriority,w:unhideWhenUsed</t>
         </is>
@@ -855,20 +875,25 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
+          <t>core</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
           <t>docapi:insert</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>No (if target omitted)</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>When target is omitted, inserts at default insertion point; can seed content from blank.</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -946,19 +971,19 @@
 </t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-insert-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:insert</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
+      <c r="H5" s="2" t="inlineStr">
         <is>
           <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numbering,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
-      <c r="H5" s="2" t="inlineStr">
+      <c r="I5" s="2" t="inlineStr">
         <is>
           <t>Properties,w:basedOn,w:color,w:ind,w:name,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
@@ -972,20 +997,25 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
+          <t>lists</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
           <t>docapi:lists-insert</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Requires existing list item target (ListItemAddress). Script seeds first list item before calling lists.insert.</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -1078,19 +1108,19 @@
 </t>
         </is>
       </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-lists-insert-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-insert</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>Properties,lpwstr,w:abstractNum,w:abstractNumId,w:basedOn,w:color,w:ilvl,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:name,w:nsid,w:num,w:numFmt,w:numId,w:numPr,w:numbering,w:p,w:pPr,w:r,w:rFonts,w:rPr,w:rsid,w:start,w:style,w:t,w:tmpl,w:u,w:uiPriority,w:unhideWhenUsed</t>
         </is>
       </c>
-      <c r="H6" s="2" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>Properties,w:basedOn,w:body,w:color,w:ilvl,w:ind,w:name,w:numPr,w:p,w:pPr,w:rFonts,w:rPr,w:rsid,w:style,w:styles,w:uiPriority,w:unhideWhenUsed</t>
         </is>
@@ -1104,20 +1134,25 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
+          <t>core</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
           <t>docapi:replace</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -1345,19 +1380,19 @@
 </t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-replace-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:replace</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H7" s="2" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
         <is>
           <t>w:t</t>
         </is>
@@ -1371,20 +1406,25 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
+          <t>core</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
           <t>docapi:delete</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -1612,19 +1652,19 @@
 </t>
         </is>
       </c>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="G8" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-delete-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:delete</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
+      <c r="H8" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H8" s="2" t="inlineStr">
+      <c r="I8" s="2" t="inlineStr">
         <is>
           <t>w:t</t>
         </is>
@@ -1638,20 +1678,25 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
           <t>docapi:blocks-delete</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Requires existing block target (heading/paragraph/table/etc).</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -1879,19 +1924,19 @@
 </t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="G9" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-heading-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-blocks-delete-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:blocks-delete</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
+      <c r="H9" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
+      <c r="I9" s="2" t="inlineStr">
         <is>
           <t>w:body,w:p,w:pPr</t>
         </is>
@@ -1905,20 +1950,25 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
           <t>docapi:format-apply</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -2146,19 +2196,19 @@
 </t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
+      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-format-apply-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:format-apply</t>
         </is>
       </c>
-      <c r="G10" s="2" t="inlineStr">
+      <c r="H10" s="2" t="inlineStr">
         <is>
           <t>w:b,w:r,w:rPr,w:t</t>
         </is>
       </c>
-      <c r="H10" s="2" t="inlineStr">
+      <c r="I10" s="2" t="inlineStr">
         <is>
           <t>w:b,w:p,w:r,w:rPr,w:t</t>
         </is>
@@ -2172,20 +2222,25 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
           <t>docapi:format-font-size</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -2413,19 +2468,19 @@
 </t>
         </is>
       </c>
-      <c r="F11" s="2" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-format-font-size-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:format-font-size</t>
         </is>
       </c>
-      <c r="G11" s="2" t="inlineStr">
+      <c r="H11" s="2" t="inlineStr">
         <is>
           <t>w:r,w:rPr,w:sz,w:t</t>
         </is>
       </c>
-      <c r="H11" s="2" t="inlineStr">
+      <c r="I11" s="2" t="inlineStr">
         <is>
           <t>w:p,w:r,w:rPr,w:sz,w:t</t>
         </is>
@@ -2439,20 +2494,25 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
           <t>docapi:format-font-family</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -2680,19 +2740,19 @@
 </t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-format-font-family-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:format-font-family</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr">
+      <c r="H12" s="2" t="inlineStr">
         <is>
           <t>w:r,w:rFonts,w:rPr,w:t</t>
         </is>
       </c>
-      <c r="H12" s="2" t="inlineStr">
+      <c r="I12" s="2" t="inlineStr">
         <is>
           <t>w:p,w:r,w:rFonts,w:rPr,w:t</t>
         </is>
@@ -2706,20 +2766,25 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
           <t>docapi:format-color</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -2947,19 +3012,19 @@
 </t>
         </is>
       </c>
-      <c r="F13" s="2" t="inlineStr">
+      <c r="G13" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-format-color-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:format-color</t>
         </is>
       </c>
-      <c r="G13" s="2" t="inlineStr">
+      <c r="H13" s="2" t="inlineStr">
         <is>
           <t>w:color,w:r,w:rPr,w:t</t>
         </is>
       </c>
-      <c r="H13" s="2" t="inlineStr">
+      <c r="I13" s="2" t="inlineStr">
         <is>
           <t>w:color,w:p,w:r,w:rPr,w:t</t>
         </is>
@@ -2973,20 +3038,25 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
           <t>docapi:format-align</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target.</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -3214,19 +3284,19 @@
 </t>
         </is>
       </c>
-      <c r="F14" s="2" t="inlineStr">
+      <c r="G14" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-format-align-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:format-align</t>
         </is>
       </c>
-      <c r="G14" s="2" t="inlineStr">
+      <c r="H14" s="2" t="inlineStr">
         <is>
           <t>w:jc,w:pPr</t>
         </is>
       </c>
-      <c r="H14" s="2" t="inlineStr">
+      <c r="I14" s="2" t="inlineStr">
         <is>
           <t>w:jc,w:p,w:pPr</t>
         </is>
@@ -3240,20 +3310,25 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
           <t>docapi:comments-create</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>Requires existing text target for root comment.</t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -3481,19 +3556,19 @@
 </t>
         </is>
       </c>
-      <c r="F15" s="2" t="inlineStr">
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-comments-create-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:comments-create</t>
         </is>
       </c>
-      <c r="G15" s="2" t="inlineStr">
+      <c r="H15" s="2" t="inlineStr">
         <is>
           <t>ct:Override,w:annotationRef,w:comment,w:commentRangeEnd,w:commentRangeStart,w:commentReference,w:comments,w:p,w:r,w:rPr,w:rStyle,w:t</t>
         </is>
       </c>
-      <c r="H15" s="2" t="inlineStr">
+      <c r="I15" s="2" t="inlineStr">
         <is>
           <t>ct:Override,ct:Types,w:p,w:r,w:rPr,w:t</t>
         </is>
@@ -3507,20 +3582,25 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
           <t>docapi:comments-patch</t>
         </is>
       </c>
-      <c r="C16" s="2" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>Requires existing comment target (script creates one first).</t>
         </is>
       </c>
-      <c r="E16" s="2" t="inlineStr">
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -3748,19 +3828,19 @@
 </t>
         </is>
       </c>
-      <c r="F16" s="2" t="inlineStr">
+      <c r="G16" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-comments-patch-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:comments-patch</t>
         </is>
       </c>
-      <c r="G16" s="2" t="inlineStr">
+      <c r="H16" s="2" t="inlineStr">
         <is>
           <t>ct:Override,w:annotationRef,w:comment,w:commentRangeEnd,w:commentRangeStart,w:commentReference,w:comments,w:p,w:r,w:rPr,w:rStyle,w:t</t>
         </is>
       </c>
-      <c r="H16" s="2" t="inlineStr">
+      <c r="I16" s="2" t="inlineStr">
         <is>
           <t>ct:Override,ct:Types,w:p,w:r,w:rPr,w:t</t>
         </is>
@@ -3774,20 +3854,25 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
           <t>docapi:comments-delete</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="E17" s="2" t="inlineStr">
         <is>
           <t>Requires existing comment target (script creates one first).</t>
         </is>
       </c>
-      <c r="E17" s="2" t="inlineStr">
+      <c r="F17" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -4015,19 +4100,19 @@
 </t>
         </is>
       </c>
-      <c r="F17" s="2" t="inlineStr">
+      <c r="G17" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-paragraph-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-comments-delete-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:comments-delete</t>
         </is>
       </c>
-      <c r="G17" s="2" t="inlineStr">
+      <c r="H17" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H17" s="2" t="inlineStr">
+      <c r="I17" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4041,20 +4126,25 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
+          <t>lists</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
           <t>docapi:lists-set-type</t>
         </is>
       </c>
-      <c r="C18" s="2" t="inlineStr">
+      <c r="D18" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="E18" s="2" t="inlineStr">
         <is>
           <t>Requires existing list item target.</t>
         </is>
       </c>
-      <c r="E18" s="2" t="inlineStr">
+      <c r="F18" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -4282,19 +4372,19 @@
 </t>
         </is>
       </c>
-      <c r="F18" s="2" t="inlineStr">
+      <c r="G18" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Output/docapi-lists-insert-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-lists-set-type-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-set-type</t>
         </is>
       </c>
-      <c r="G18" s="2" t="inlineStr">
+      <c r="H18" s="2" t="inlineStr">
         <is>
           <t>w:abstractNum,w:abstractNumId,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:nsid,w:num,w:numFmt,w:pPr,w:rFonts,w:rPr,w:start,w:tmpl</t>
         </is>
       </c>
-      <c r="H18" s="2" t="inlineStr">
+      <c r="I18" s="2" t="inlineStr">
         <is>
           <t>w:abstractNum,w:abstractNumId,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:nsid,w:num,w:numFmt,w:numId,w:numbering,w:pPr,w:rFonts,w:rPr,w:start,w:tmpl</t>
         </is>
@@ -4308,20 +4398,25 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
+          <t>lists</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
           <t>docapi:lists-indent</t>
         </is>
       </c>
-      <c r="C19" s="2" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>Requires existing list item target.</t>
         </is>
       </c>
-      <c r="E19" s="2" t="inlineStr">
+      <c r="F19" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -4549,19 +4644,19 @@
 </t>
         </is>
       </c>
-      <c r="F19" s="2" t="inlineStr">
+      <c r="G19" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Output/docapi-lists-insert-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-lists-indent-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-indent</t>
         </is>
       </c>
-      <c r="G19" s="2" t="inlineStr">
+      <c r="H19" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H19" s="2" t="inlineStr">
+      <c r="I19" s="2" t="inlineStr">
         <is>
           <t>w:ilvl</t>
         </is>
@@ -4575,20 +4670,25 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
+          <t>lists</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
           <t>docapi:lists-outdent</t>
         </is>
       </c>
-      <c r="C20" s="2" t="inlineStr">
+      <c r="D20" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr">
+      <c r="E20" s="2" t="inlineStr">
         <is>
           <t>Requires existing list item target.</t>
         </is>
       </c>
-      <c r="E20" s="2" t="inlineStr">
+      <c r="F20" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -4816,19 +4916,19 @@
 </t>
         </is>
       </c>
-      <c r="F20" s="2" t="inlineStr">
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Output/docapi-lists-insert-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-lists-outdent-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-outdent</t>
         </is>
       </c>
-      <c r="G20" s="2" t="inlineStr">
+      <c r="H20" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H20" s="2" t="inlineStr">
+      <c r="I20" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4842,20 +4942,25 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
+          <t>lists</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
           <t>docapi:lists-restart</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr">
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>Requires existing list item target.</t>
         </is>
       </c>
-      <c r="E21" s="2" t="inlineStr">
+      <c r="F21" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -5083,19 +5188,19 @@
 </t>
         </is>
       </c>
-      <c r="F21" s="2" t="inlineStr">
+      <c r="G21" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Output/docapi-lists-insert-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-lists-restart-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-restart</t>
         </is>
       </c>
-      <c r="G21" s="2" t="inlineStr">
+      <c r="H21" s="2" t="inlineStr">
         <is>
           <t>w:abstractNum,w:abstractNumId,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:num,w:numFmt,w:pPr,w:start,w:tmpl</t>
         </is>
       </c>
-      <c r="H21" s="2" t="inlineStr">
+      <c r="I21" s="2" t="inlineStr">
         <is>
           <t>w:abstractNum,w:abstractNumId,w:ind,w:lvl,w:lvlJc,w:lvlText,w:multiLevelType,w:num,w:numFmt,w:numId,w:numbering,w:pPr,w:start,w:tmpl</t>
         </is>
@@ -5109,20 +5214,25 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
+          <t>lists</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
           <t>docapi:lists-exit</t>
         </is>
       </c>
-      <c r="C22" s="2" t="inlineStr">
+      <c r="D22" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr">
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>Requires existing list item target.</t>
         </is>
       </c>
-      <c r="E22" s="2" t="inlineStr">
+      <c r="F22" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -5350,19 +5460,19 @@
 </t>
         </is>
       </c>
-      <c r="F22" s="2" t="inlineStr">
+      <c r="G22" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Output/docapi-lists-insert-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-lists-exit-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:lists-exit</t>
         </is>
       </c>
-      <c r="G22" s="2" t="inlineStr">
+      <c r="H22" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H22" s="2" t="inlineStr">
+      <c r="I22" s="2" t="inlineStr">
         <is>
           <t>w:ilvl,w:numId,w:numPr,w:p,w:pPr</t>
         </is>
@@ -5376,20 +5486,25 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
+          <t>tables</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
           <t>docapi:tables-insert-row</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>Requires existing table target.</t>
         </is>
       </c>
-      <c r="E23" s="2" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -5617,19 +5732,19 @@
 </t>
         </is>
       </c>
-      <c r="F23" s="2" t="inlineStr">
+      <c r="G23" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-table-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-tables-insert-row-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:tables-insert-row</t>
         </is>
       </c>
-      <c r="G23" s="2" t="inlineStr">
+      <c r="H23" s="2" t="inlineStr">
         <is>
           <t>w:bottom,w:left,w:p,w:right,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr</t>
         </is>
       </c>
-      <c r="H23" s="2" t="inlineStr">
+      <c r="I23" s="2" t="inlineStr">
         <is>
           <t>w:bottom,w:left,w:p,w:right,w:tbl,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr</t>
         </is>
@@ -5643,20 +5758,25 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
+          <t>tables</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
           <t>docapi:tables-delete-row</t>
         </is>
       </c>
-      <c r="C24" s="2" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr">
+      <c r="E24" s="2" t="inlineStr">
         <is>
           <t>Requires existing table target.</t>
         </is>
       </c>
-      <c r="E24" s="2" t="inlineStr">
+      <c r="F24" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -5884,19 +6004,19 @@
 </t>
         </is>
       </c>
-      <c r="F24" s="2" t="inlineStr">
+      <c r="G24" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-table-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-tables-delete-row-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:tables-delete-row</t>
         </is>
       </c>
-      <c r="G24" s="2" t="inlineStr">
+      <c r="H24" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H24" s="2" t="inlineStr">
+      <c r="I24" s="2" t="inlineStr">
         <is>
           <t>w:bottom,w:left,w:p,w:right,w:tbl,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr</t>
         </is>
@@ -5910,20 +6030,25 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
+          <t>tables</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
           <t>docapi:tables-insert-column</t>
         </is>
       </c>
-      <c r="C25" s="2" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D25" s="2" t="inlineStr">
+      <c r="E25" s="2" t="inlineStr">
         <is>
           <t>Requires existing table target.</t>
         </is>
       </c>
-      <c r="E25" s="2" t="inlineStr">
+      <c r="F25" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -6151,19 +6276,19 @@
 </t>
         </is>
       </c>
-      <c r="F25" s="2" t="inlineStr">
+      <c r="G25" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-table-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-tables-insert-column-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:tables-insert-column</t>
         </is>
       </c>
-      <c r="G25" s="2" t="inlineStr">
+      <c r="H25" s="2" t="inlineStr">
         <is>
           <t>w:bottom,w:gridCol,w:left,w:p,w:right,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top</t>
         </is>
       </c>
-      <c r="H25" s="2" t="inlineStr">
+      <c r="I25" s="2" t="inlineStr">
         <is>
           <t>w:bottom,w:gridCol,w:left,w:p,w:right,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr</t>
         </is>
@@ -6177,20 +6302,25 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
+          <t>tables</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
           <t>docapi:tables-delete-column</t>
         </is>
       </c>
-      <c r="C26" s="2" t="inlineStr">
+      <c r="D26" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D26" s="2" t="inlineStr">
+      <c r="E26" s="2" t="inlineStr">
         <is>
           <t>Requires existing table target.</t>
         </is>
       </c>
-      <c r="E26" s="2" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">import { mkdir, stat } from 'node:fs/promises';
 import { dirname } from 'node:path';
@@ -6418,19 +6548,19 @@
 </t>
         </is>
       </c>
-      <c r="F26" s="2" t="inlineStr">
+      <c r="G26" s="2" t="inlineStr">
         <is>
           <t>DOCAPI_SOURCE="https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/docapi-create-table-output.docx" \
 DOCAPI_OUTPUT="/Users/missyresutko/Documents/Codex/Github/temp-doc-host/Output/docapi-tables-delete-column-output.docx" \
 pnpm --dir /Users/missyresutko/Documents/Codex/SuperDoc/repo run docapi:tables-delete-column</t>
         </is>
       </c>
-      <c r="G26" s="2" t="inlineStr">
+      <c r="H26" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H26" s="2" t="inlineStr">
+      <c r="I26" s="2" t="inlineStr">
         <is>
           <t>w:bottom,w:gridCol,w:left,w:p,w:right,w:tblGrid,w:tc,w:tcBorders,w:tcPr,w:tcW,w:top,w:tr</t>
         </is>

</xml_diff>

<commit_message>
Regenerate docapi workbook and rerun all output fixtures
</commit_message>
<xml_diff>
--- a/docapi-create-operations.xlsx
+++ b/docapi-create-operations.xlsx
@@ -49,7 +49,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
@@ -57,7 +57,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,13 +431,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="26" customWidth="1" min="3" max="3"/>
-    <col width="52" customWidth="1" min="4" max="4"/>
-    <col width="110" customWidth="1" min="5" max="5"/>
-    <col width="95" customWidth="1" min="6" max="6"/>
-    <col width="70" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="26" customWidth="1" min="4" max="4"/>
+    <col width="52" customWidth="1" min="5" max="5"/>
+    <col width="110" customWidth="1" min="6" max="6"/>
+    <col width="95" customWidth="1" min="7" max="7"/>
     <col width="70" customWidth="1" min="8" max="8"/>
+    <col width="70" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -526,9 +526,7 @@
 import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
 function toRawGithubUrl(input: string): string {
   if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
+  return input.replace('https://github.com/', 'https://raw.githubusercontent.com/').replace('/blob/', '/');
 }
 function isHttpSource(input: string): boolean {
   return input.startsWith('http://') || input.startsWith('https://');
@@ -565,8 +563,7 @@
 }
 describe('docapi create paragraph', () =&gt; {
   it('creates a paragraph via create.paragraph and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
+    const source = process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
     const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-create-paragraph-output.docx';
     const paragraphText = process.env.DOCAPI_PARAGRAPH_TEXT ?? 'apples, bananas, mangoes';
     await mkdir(dirname(outputPath), { recursive: true });
@@ -650,9 +647,7 @@
 import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
 function toRawGithubUrl(input: string): string {
   if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
+  return input.replace('https://github.com/', 'https://raw.githubusercontent.com/').replace('/blob/', '/');
 }
 function isHttpSource(input: string): boolean {
   return input.startsWith('http://') || input.startsWith('https://');
@@ -689,8 +684,7 @@
 }
 describe('docapi create heading', () =&gt; {
   it('creates a heading via create.heading and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
+    const source = process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
     const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-create-heading-output.docx';
     const headingText = process.env.DOCAPI_HEADING_TEXT ?? 'FRUIT';
     const headingLevelRaw = Number.parseInt(process.env.DOCAPI_HEADING_LEVEL ?? '1', 10);
@@ -777,9 +771,7 @@
 import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
 function toRawGithubUrl(input: string): string {
   if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
+  return input.replace('https://github.com/', 'https://raw.githubusercontent.com/').replace('/blob/', '/');
 }
 function isHttpSource(input: string): boolean {
   return input.startsWith('http://') || input.startsWith('https://');
@@ -816,8 +808,7 @@
 }
 describe('docapi create table', () =&gt; {
   it('creates a table via create.table and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
+    const source = process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
     const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-create-table-output.docx';
     const rowsRaw = Number.parseInt(process.env.DOCAPI_TABLE_ROWS ?? '3', 10);
     const columnsRaw = Number.parseInt(process.env.DOCAPI_TABLE_COLUMNS ?? '3', 10);
@@ -905,9 +896,7 @@
 import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
 function toRawGithubUrl(input: string): string {
   if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
+  return input.replace('https://github.com/', 'https://raw.githubusercontent.com/').replace('/blob/', '/');
 }
 function isHttpSource(input: string): boolean {
   return input.startsWith('http://') || input.startsWith('https://');
@@ -944,8 +933,7 @@
 }
 describe('docapi insert', () =&gt; {
   it('seeds content via insert and exports docx', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
+    const source = process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
     const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-insert-output.docx';
     const insertText = process.env.DOCAPI_INSERT_TEXT ?? 'Seed content for follow-up operations.';
     await mkdir(dirname(outputPath), { recursive: true });
@@ -1027,9 +1015,7 @@
 import { assembleDocumentApiAdapters } from '../document-api-adapters/assemble-adapters.js';
 function toRawGithubUrl(input: string): string {
   if (!input.includes('github.com') || !input.includes('/blob/')) return input;
-  return input
-    .replace('https://github.com/', 'https://raw.githubusercontent.com/')
-    .replace('/blob/', '/');
+  return input.replace('https://github.com/', 'https://raw.githubusercontent.com/').replace('/blob/', '/');
 }
 function isHttpSource(input: string): boolean {
   return input.startsWith('http://') || input.startsWith('https://');
@@ -1066,8 +1052,7 @@
 }
 describe('docapi lists.insert', () =&gt; {
   it('inserts a list item after seeding an initial list item target', async () =&gt; {
-    const source =
-      process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
+    const source = process.env.DOCAPI_SOURCE ?? 'https://github.com/missysuperdoc/temp-doc-host/blob/main/Blank.docx';
     const outputPath = process.env.DOCAPI_OUTPUT ?? '/Users/missyresutko/Downloads/docapi-lists-insert-output.docx';
     const firstItemText = process.env.DOCAPI_LIST_SEED_TEXT ?? 'Yabba';
     const insertedItemText = process.env.DOCAPI_ITEM_TEXT ?? 'Dabba';
@@ -1225,8 +1210,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -1260,13 +1244,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -1317,7 +1307,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -1341,7 +1334,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -1497,8 +1493,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -1532,13 +1527,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -1589,7 +1590,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -1613,7 +1617,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -1769,8 +1776,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -1804,13 +1810,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -1861,7 +1873,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -1885,7 +1900,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -2041,8 +2059,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -2076,13 +2093,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -2133,7 +2156,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -2157,7 +2183,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -2313,8 +2342,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -2348,13 +2376,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -2405,7 +2439,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -2429,7 +2466,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -2585,8 +2625,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -2620,13 +2659,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -2677,7 +2722,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -2701,7 +2749,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -2857,8 +2908,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -2892,13 +2942,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -2949,7 +3005,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -2973,7 +3032,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -3129,8 +3191,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -3164,13 +3225,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -3221,7 +3288,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -3245,7 +3315,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -3401,8 +3474,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -3436,13 +3508,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -3493,7 +3571,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -3517,7 +3598,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -3673,8 +3757,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -3708,13 +3791,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -3765,7 +3854,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -3789,7 +3881,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -3945,8 +4040,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -3980,13 +4074,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -4037,7 +4137,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -4061,7 +4164,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -4217,8 +4323,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -4252,13 +4357,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -4309,7 +4420,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -4333,7 +4447,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -4489,8 +4606,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -4524,13 +4640,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -4581,7 +4703,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -4605,7 +4730,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -4761,8 +4889,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -4796,13 +4923,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -4853,7 +4986,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -4877,7 +5013,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -5033,8 +5172,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -5068,13 +5206,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -5125,7 +5269,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -5149,7 +5296,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -5305,8 +5455,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -5340,13 +5489,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -5397,7 +5552,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -5421,7 +5579,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -5577,8 +5738,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -5612,13 +5772,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -5669,7 +5835,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -5693,7 +5862,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -5849,8 +6021,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -5884,13 +6055,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -5941,7 +6118,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -5965,7 +6145,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -6121,8 +6304,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -6156,13 +6338,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -6213,7 +6401,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -6237,7 +6428,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {
@@ -6393,8 +6587,7 @@
       process.env.DOCAPI_SOURCE ??
       'https://github.com/missysuperdoc/temp-doc-host/blob/main/Starting%20files/Blank.docx';
     const outputPath =
-      process.env.DOCAPI_OUTPUT ??
-      `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
+      process.env.DOCAPI_OUTPUT ?? `/Users/missyresutko/Downloads/docapi-${operation.replaceAll('.', '-')}-output.docx`;
     await mkdir(dirname(outputPath), { recursive: true });
     const openedSource = await loadSource(source);
     const editor = await Editor.open(openedSource, { mode: 'docx', isHeadless: true });
@@ -6428,13 +6621,19 @@
         case 'format.fontSize': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontSize requires a text target.');
-          requireSuccess(doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }), operation);
+          requireSuccess(
+            doc.format.fontSize({ target, value: Number(process.env.DOCAPI_FONT_SIZE ?? '18') }),
+            operation,
+          );
           break;
         }
         case 'format.fontFamily': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('format.fontFamily requires a text target.');
-          requireSuccess(doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }), operation);
+          requireSuccess(
+            doc.format.fontFamily({ target, value: process.env.DOCAPI_FONT_FAMILY ?? 'Arial' }),
+            operation,
+          );
           break;
         }
         case 'format.color': {
@@ -6485,7 +6684,10 @@
         case 'comments.create': {
           const target = firstTextRange(doc);
           if (!target) throw new Error('comments.create requires a text target.');
-          requireSuccess(doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }), operation);
+          requireSuccess(
+            doc.comments.create({ target, text: process.env.DOCAPI_COMMENT_TEXT ?? 'is this compliant?' }),
+            operation,
+          );
           break;
         }
         case 'comments.patch': {
@@ -6509,7 +6711,10 @@
         case 'tables.insertRow': {
           const table = firstNodeAddress(doc, 'table');
           if (!table) throw new Error('tables.insertRow requires a table.');
-          requireSuccess(doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }), operation);
+          requireSuccess(
+            doc.tables.insertRow({ tableTarget: table as never, rowIndex: 0, position: 'below', count: 1 }),
+            operation,
+          );
           break;
         }
         case 'tables.deleteRow': {

</xml_diff>